<commit_message>
0.0.17: packageSuffix and overridePackage option is now available.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtClassStructure.xlsx
+++ b/meta/program/BlancoValueObjectKtClassStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4230F327-F5BE-3141-8946-58DD5D2C836E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A7D506-D72A-2649-A014-38A46087F78A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="560" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -446,6 +446,43 @@
     <t>委譲を記憶するリストを指定します。</t>
     <rPh sb="0" eb="2">
       <t xml:space="preserve">イジョウ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>packageSuffix</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>パッケージ名の後ろに付加する文字列をしていします。</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">パッケージメイ </t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t xml:space="preserve">ウシロニ </t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t xml:space="preserve">フカ </t>
+    </rPh>
+    <rPh sb="14" eb="17">
+      <t xml:space="preserve">モジレツ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>overridePackage</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>定義書で指定されたパッケージ名を上書きします。</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">テイギショ </t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t xml:space="preserve">シテイ </t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t xml:space="preserve">ウワガキシマス。 </t>
     </rPh>
     <phoneticPr fontId="3"/>
   </si>
@@ -987,35 +1024,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1427,10 +1464,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45:F45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1625,24 +1662,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="54"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="56"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="56"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="54"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="56"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1684,30 +1721,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E25" s="50" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="56"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1748,7 +1785,7 @@
     </row>
     <row r="29" spans="1:7" ht="15">
       <c r="A29" s="38">
-        <f t="shared" ref="A29:A46" si="0">A28+1</f>
+        <f t="shared" ref="A29:A49" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -1796,10 +1833,10 @@
       <c r="D31" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="51" t="s">
+      <c r="E31" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="52"/>
+      <c r="F31" s="54"/>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="15">
@@ -1816,10 +1853,10 @@
       <c r="D32" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="51" t="s">
+      <c r="E32" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="54"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="15">
@@ -1836,10 +1873,10 @@
       <c r="D33" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="51" t="s">
+      <c r="E33" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="52"/>
+      <c r="F33" s="54"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15">
@@ -1856,10 +1893,10 @@
       <c r="D34" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="E34" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="52"/>
+      <c r="F34" s="54"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15">
@@ -1876,10 +1913,10 @@
       <c r="D35" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="51" t="s">
+      <c r="E35" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="F35" s="52"/>
+      <c r="F35" s="54"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="15">
@@ -1896,10 +1933,10 @@
       <c r="D36" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="52"/>
+      <c r="F36" s="54"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -1916,10 +1953,10 @@
       <c r="D37" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="51" t="s">
+      <c r="E37" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="52"/>
+      <c r="F37" s="54"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -1936,10 +1973,10 @@
       <c r="D38" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="51" t="s">
+      <c r="E38" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="52"/>
+      <c r="F38" s="54"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="15">
@@ -1956,10 +1993,10 @@
       <c r="D39" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="51" t="s">
+      <c r="E39" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="F39" s="52"/>
+      <c r="F39" s="54"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="15">
@@ -1976,10 +2013,10 @@
       <c r="D40" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="51" t="s">
+      <c r="E40" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="52"/>
+      <c r="F40" s="54"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="15">
@@ -1994,10 +2031,10 @@
         <v>33</v>
       </c>
       <c r="D41" s="40"/>
-      <c r="E41" s="51" t="s">
+      <c r="E41" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="F41" s="52"/>
+      <c r="F41" s="54"/>
       <c r="G41"/>
     </row>
     <row r="42" spans="1:7" ht="45" customHeight="1">
@@ -2014,10 +2051,10 @@
       <c r="D42" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="51" t="s">
+      <c r="E42" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="53"/>
+      <c r="F42" s="55"/>
       <c r="G42"/>
     </row>
     <row r="43" spans="1:7" ht="45">
@@ -2034,10 +2071,10 @@
       <c r="D43" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="E43" s="51" t="s">
+      <c r="E43" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="F43" s="53"/>
+      <c r="F43" s="55"/>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:7" ht="45">
@@ -2054,10 +2091,10 @@
       <c r="D44" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="51" t="s">
+      <c r="E44" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="F44" s="53"/>
+      <c r="F44" s="55"/>
       <c r="G44"/>
     </row>
     <row r="45" spans="1:7" ht="15">
@@ -2072,10 +2109,10 @@
         <v>63</v>
       </c>
       <c r="D45" s="40"/>
-      <c r="E45" s="51" t="s">
+      <c r="E45" s="53" t="s">
         <v>62</v>
       </c>
-      <c r="F45" s="53"/>
+      <c r="F45" s="55"/>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7">
@@ -2092,34 +2129,84 @@
       <c r="D46" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="E46" s="51" t="s">
+      <c r="E46" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="F46" s="52"/>
+      <c r="F46" s="54"/>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:7" ht="14" customHeight="1">
-      <c r="A47" s="21"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="50"/>
+    <row r="47" spans="1:7" ht="15">
+      <c r="A47" s="38">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B47" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="45"/>
+      <c r="E47" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="54"/>
       <c r="G47"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" ht="15">
+      <c r="A48" s="38">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B48" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="45"/>
+      <c r="E48" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="F48" s="54"/>
       <c r="G48"/>
     </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="38"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="54"/>
+      <c r="G49"/>
+    </row>
+    <row r="50" spans="1:7" ht="14" customHeight="1">
+      <c r="A50" s="21"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="57"/>
+      <c r="F50" s="58"/>
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="G51"/>
+    </row>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
+  <mergeCells count="30">
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E48:F48"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="E42:F42"/>
     <mergeCell ref="E19:E20"/>
@@ -2129,20 +2216,18 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D61" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D64" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
0.1.8: Now enable to generate enum class.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtClassStructure.xlsx
+++ b/meta/program/BlancoValueObjectKtClassStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD8C98E-DA9E-6F44-A588-36512A4AB56C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC38BF0-A929-1148-9CB2-06B229FEEAF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14540" yWindow="3820" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <definedName name="項目型">#REF!</definedName>
     <definedName name="必須">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -492,6 +492,20 @@
   </si>
   <si>
     <t>new blanco.valueobjectkt.valueobject.BlancoValueObjectKtExtendsStructure()</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>enumeration</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>列挙型として定義します。</t>
+    <rPh sb="0" eb="3">
+      <t xml:space="preserve">レッキョガタ </t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t xml:space="preserve">テイギ </t>
+    </rPh>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1032,35 +1046,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1472,10 +1486,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41:F41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43:F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1670,24 +1684,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="54"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="56"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="56"/>
-      <c r="B20" s="57"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="54"/>
+      <c r="A20" s="49"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="56"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1729,30 +1743,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="56" t="s">
+      <c r="A25" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="56" t="s">
+      <c r="B25" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="55" t="s">
+      <c r="E25" s="50" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="56"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="55"/>
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1793,7 +1807,7 @@
     </row>
     <row r="29" spans="1:7" ht="15">
       <c r="A29" s="38">
-        <f t="shared" ref="A29:A48" si="0">A28+1</f>
+        <f t="shared" ref="A29:A49" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -1841,10 +1855,10 @@
       <c r="D31" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="51" t="s">
+      <c r="E31" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="52"/>
+      <c r="F31" s="54"/>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="15">
@@ -1861,10 +1875,10 @@
       <c r="D32" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="51" t="s">
+      <c r="E32" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="54"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="15">
@@ -1881,10 +1895,10 @@
       <c r="D33" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="51" t="s">
+      <c r="E33" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="52"/>
+      <c r="F33" s="54"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15">
@@ -1901,10 +1915,10 @@
       <c r="D34" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="51" t="s">
+      <c r="E34" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="52"/>
+      <c r="F34" s="54"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15">
@@ -1921,10 +1935,10 @@
       <c r="D35" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="51" t="s">
+      <c r="E35" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="F35" s="52"/>
+      <c r="F35" s="54"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="15">
@@ -1941,10 +1955,10 @@
       <c r="D36" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="F36" s="52"/>
+      <c r="F36" s="54"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -1961,10 +1975,10 @@
       <c r="D37" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E37" s="51" t="s">
+      <c r="E37" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="52"/>
+      <c r="F37" s="54"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -1981,10 +1995,10 @@
       <c r="D38" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="51" t="s">
+      <c r="E38" s="53" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="52"/>
+      <c r="F38" s="54"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="15">
@@ -2001,16 +2015,16 @@
       <c r="D39" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="51" t="s">
+      <c r="E39" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="F39" s="52"/>
+      <c r="F39" s="54"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="15">
       <c r="A40" s="38">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f>A38+1</f>
+        <v>13</v>
       </c>
       <c r="B40" s="39" t="s">
         <v>49</v>
@@ -2021,189 +2035,232 @@
       <c r="D40" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="51" t="s">
+      <c r="E40" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="52"/>
+      <c r="F40" s="54"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="1:7" ht="45">
+    <row r="41" spans="1:7" ht="15">
       <c r="A41" s="38">
+        <f>A39+1</f>
+        <v>14</v>
+      </c>
+      <c r="B41" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="F41" s="54"/>
+      <c r="G41"/>
+    </row>
+    <row r="42" spans="1:7" ht="45">
+      <c r="A42" s="38">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B41" s="39" t="s">
+      <c r="B42" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C42" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D42" s="40" t="s">
         <v>93</v>
       </c>
-      <c r="E41" s="51" t="s">
+      <c r="E42" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="F41" s="52"/>
-      <c r="G41"/>
-    </row>
-    <row r="42" spans="1:7" ht="45" customHeight="1">
-      <c r="A42" s="38">
+      <c r="F42" s="54"/>
+      <c r="G42"/>
+    </row>
+    <row r="43" spans="1:7" ht="45" customHeight="1">
+      <c r="A43" s="38">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B42" s="39" t="s">
+      <c r="B43" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C43" s="40" t="s">
         <v>56</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D43" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E42" s="51" t="s">
+      <c r="E43" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F42" s="53"/>
-      <c r="G42"/>
-    </row>
-    <row r="43" spans="1:7" ht="45">
-      <c r="A43" s="38">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B43" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C43" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="E43" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="F43" s="53"/>
+      <c r="F43" s="55"/>
       <c r="G43"/>
     </row>
     <row r="44" spans="1:7" ht="45">
       <c r="A44" s="38">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B44" s="39" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D44" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="E44" s="51" t="s">
-        <v>87</v>
-      </c>
-      <c r="F44" s="53"/>
+        <v>72</v>
+      </c>
+      <c r="E44" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="F44" s="55"/>
       <c r="G44"/>
     </row>
-    <row r="45" spans="1:7" ht="15">
+    <row r="45" spans="1:7" ht="45">
       <c r="A45" s="38">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C45" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D45" s="40"/>
-      <c r="E45" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="F45" s="53"/>
+        <v>85</v>
+      </c>
+      <c r="D45" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="F45" s="55"/>
       <c r="G45"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" ht="15">
       <c r="A46" s="38">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B46" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="D46" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="E46" s="51" t="s">
-        <v>78</v>
-      </c>
-      <c r="F46" s="52"/>
+        <v>19</v>
+      </c>
+      <c r="B46" s="39" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="40"/>
+      <c r="E46" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="F46" s="55"/>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:7" ht="15">
+    <row r="47" spans="1:7">
       <c r="A47" s="38">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B47" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C47" s="40" t="s">
-        <v>63</v>
-      </c>
-      <c r="D47" s="45"/>
-      <c r="E47" s="51" t="s">
-        <v>89</v>
-      </c>
-      <c r="F47" s="52"/>
+        <v>75</v>
+      </c>
+      <c r="C47" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="53" t="s">
+        <v>78</v>
+      </c>
+      <c r="F47" s="54"/>
       <c r="G47"/>
     </row>
     <row r="48" spans="1:7" ht="15">
       <c r="A48" s="38">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B48" s="44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C48" s="40" t="s">
         <v>63</v>
       </c>
       <c r="D48" s="45"/>
-      <c r="E48" s="51" t="s">
+      <c r="E48" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="F48" s="54"/>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="1:7" ht="15">
+      <c r="A49" s="38">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B49" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="45"/>
+      <c r="E49" s="53" t="s">
         <v>91</v>
       </c>
-      <c r="F48" s="52"/>
-      <c r="G48"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="38"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="51"/>
-      <c r="F49" s="52"/>
+      <c r="F49" s="54"/>
       <c r="G49"/>
     </row>
-    <row r="50" spans="1:7" ht="14" customHeight="1">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="43"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="50"/>
+    <row r="50" spans="1:7">
+      <c r="A50" s="38"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="54"/>
       <c r="G50"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" ht="14" customHeight="1">
+      <c r="A51" s="21"/>
+      <c r="B51" s="22"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="58"/>
       <c r="G51"/>
     </row>
+    <row r="52" spans="1:7">
+      <c r="G52"/>
+    </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="31">
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E44:F44"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
@@ -2212,32 +2269,10 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E48:F48"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D64" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D65" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
3.0.13 Adapt "sealed class".
</commit_message>
<xml_diff>
--- a/meta/program/BlancoValueObjectKtClassStructure.xlsx
+++ b/meta/program/BlancoValueObjectKtClassStructure.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoValueObjectKt/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5602D894-BCB2-AD4D-8EEE-33D2952C9973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1010B70-1264-CF44-A7D5-D2409B93BC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="3820" windowWidth="28300" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="100">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -514,6 +514,14 @@
   </si>
   <si>
     <t>primary constructor に @JsonCreator を指定する。コンストラクタ引数には @JsonProperty を自動付与する（別名優先）</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>sealed</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>sealedクラスかどうか。</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1052,35 +1060,35 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1492,10 +1500,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51:F51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1690,24 +1698,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="52"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="54"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="54"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="52"/>
+      <c r="A20" s="47"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="54"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1749,30 +1757,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="54" t="s">
+      <c r="B25" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="53" t="s">
+      <c r="C25" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D25" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="48" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="23"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="54"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="8"/>
       <c r="G26"/>
     </row>
@@ -1813,7 +1821,7 @@
     </row>
     <row r="29" spans="1:7" ht="15">
       <c r="A29" s="36">
-        <f t="shared" ref="A29:A50" si="0">A28+1</f>
+        <f t="shared" ref="A29:A51" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="37" t="s">
@@ -1861,10 +1869,10 @@
       <c r="D31" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E31" s="49" t="s">
+      <c r="E31" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="F31" s="50"/>
+      <c r="F31" s="52"/>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="15">
@@ -1881,10 +1889,10 @@
       <c r="D32" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="50"/>
+      <c r="F32" s="52"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="15">
@@ -1901,10 +1909,10 @@
       <c r="D33" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="F33" s="50"/>
+      <c r="F33" s="52"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="15">
@@ -1921,10 +1929,10 @@
       <c r="D34" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="49" t="s">
+      <c r="E34" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F34" s="50"/>
+      <c r="F34" s="52"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15">
@@ -1941,10 +1949,10 @@
       <c r="D35" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E35" s="49" t="s">
+      <c r="E35" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="F35" s="50"/>
+      <c r="F35" s="52"/>
       <c r="G35"/>
     </row>
     <row r="36" spans="1:7" ht="15">
@@ -1953,7 +1961,7 @@
         <v>10</v>
       </c>
       <c r="B36" s="37" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="C36" s="38" t="s">
         <v>81</v>
@@ -1961,10 +1969,10 @@
       <c r="D36" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="F36" s="50"/>
+      <c r="E36" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" s="52"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -1973,18 +1981,18 @@
         <v>11</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="C37" s="38" t="s">
         <v>81</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="50"/>
+        <v>45</v>
+      </c>
+      <c r="E37" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="52"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -1993,18 +2001,18 @@
         <v>12</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C38" s="38" t="s">
         <v>81</v>
       </c>
       <c r="D38" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="E38" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="F38" s="50"/>
+        <v>42</v>
+      </c>
+      <c r="E38" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="52"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="15">
@@ -2013,7 +2021,7 @@
         <v>13</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C39" s="38" t="s">
         <v>81</v>
@@ -2021,19 +2029,19 @@
       <c r="D39" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="F39" s="50"/>
+      <c r="E39" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="52"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="15">
       <c r="A40" s="36">
-        <f>A38+1</f>
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C40" s="38" t="s">
         <v>81</v>
@@ -2041,229 +2049,274 @@
       <c r="D40" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E40" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" s="50"/>
+      <c r="E40" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" s="52"/>
       <c r="G40"/>
     </row>
     <row r="41" spans="1:7" ht="15">
       <c r="A41" s="36">
-        <f>A39+1</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>94</v>
+        <v>49</v>
       </c>
       <c r="C41" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="38" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="F41" s="50"/>
+      <c r="D41" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="E41" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41" s="52"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="1:7" ht="45">
+    <row r="42" spans="1:7" ht="15">
       <c r="A42" s="36">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B42" s="37" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="C42" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="D42" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="E42" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" s="50"/>
+        <v>81</v>
+      </c>
+      <c r="D42" s="38" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="52"/>
       <c r="G42"/>
     </row>
-    <row r="43" spans="1:7" ht="45" customHeight="1">
+    <row r="43" spans="1:7" ht="45">
       <c r="A43" s="36">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="D43" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="F43" s="51"/>
+        <v>93</v>
+      </c>
+      <c r="E43" s="51" t="s">
+        <v>51</v>
+      </c>
+      <c r="F43" s="52"/>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:7" ht="45">
+    <row r="44" spans="1:7" ht="45" customHeight="1">
       <c r="A44" s="36">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B44" s="37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C44" s="38" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D44" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="E44" s="49" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" s="51"/>
+        <v>57</v>
+      </c>
+      <c r="E44" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="53"/>
       <c r="G44"/>
     </row>
     <row r="45" spans="1:7" ht="45">
       <c r="A45" s="36">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B45" s="37" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="C45" s="38" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D45" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="E45" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="F45" s="51"/>
+        <v>72</v>
+      </c>
+      <c r="E45" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="F45" s="53"/>
       <c r="G45"/>
     </row>
-    <row r="46" spans="1:7" ht="15">
+    <row r="46" spans="1:7" ht="45">
       <c r="A46" s="36">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C46" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="38"/>
-      <c r="E46" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="F46" s="51"/>
+        <v>85</v>
+      </c>
+      <c r="D46" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" s="51" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="53"/>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" ht="15">
       <c r="A47" s="36">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B47" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="43" t="s">
-        <v>76</v>
-      </c>
-      <c r="D47" s="43" t="s">
-        <v>77</v>
-      </c>
-      <c r="E47" s="49" t="s">
-        <v>78</v>
-      </c>
-      <c r="F47" s="50"/>
+        <v>21</v>
+      </c>
+      <c r="B47" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" s="38"/>
+      <c r="E47" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="F47" s="53"/>
       <c r="G47"/>
     </row>
-    <row r="48" spans="1:7" ht="15">
+    <row r="48" spans="1:7">
       <c r="A48" s="36">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B48" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C48" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D48" s="43"/>
-      <c r="E48" s="49" t="s">
-        <v>89</v>
-      </c>
-      <c r="F48" s="50"/>
+        <v>75</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" s="51" t="s">
+        <v>78</v>
+      </c>
+      <c r="F48" s="52"/>
       <c r="G48"/>
     </row>
     <row r="49" spans="1:7" ht="15">
       <c r="A49" s="36">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B49" s="42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C49" s="38" t="s">
         <v>63</v>
       </c>
       <c r="D49" s="43"/>
-      <c r="E49" s="49" t="s">
-        <v>91</v>
-      </c>
-      <c r="F49" s="50"/>
+      <c r="E49" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="F49" s="52"/>
       <c r="G49"/>
     </row>
     <row r="50" spans="1:7" ht="15">
       <c r="A50" s="36">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B50" s="42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" s="43"/>
+      <c r="E50" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="F50" s="52"/>
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="1:7" ht="15">
+      <c r="A51" s="36">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B51" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="C50" s="38" t="s">
+      <c r="C51" s="38" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="43" t="b">
+      <c r="D51" s="43" t="b">
         <v>0</v>
       </c>
-      <c r="E50" s="49" t="s">
+      <c r="E51" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="F50" s="50"/>
-      <c r="G50"/>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" s="36"/>
-      <c r="B51" s="42"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="50"/>
+      <c r="F51" s="52"/>
       <c r="G51"/>
     </row>
-    <row r="52" spans="1:7" ht="14" customHeight="1">
-      <c r="A52" s="20"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="41"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="48"/>
+    <row r="52" spans="1:7">
+      <c r="A52" s="36"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="38"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="51"/>
+      <c r="F52" s="52"/>
       <c r="G52"/>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" ht="14" customHeight="1">
+      <c r="A53" s="20"/>
+      <c r="B53" s="21"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="55"/>
+      <c r="F53" s="56"/>
       <c r="G53"/>
     </row>
+    <row r="54" spans="1:7">
+      <c r="G54"/>
+    </row>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="33">
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E45:F45"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
@@ -2272,34 +2325,10 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E50:F50"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations disablePrompts="1" count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D66" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D67" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>